<commit_message>
add simplified adult mouse brain
</commit_message>
<xml_diff>
--- a/Mouse/MouseAdult_CellTypes.xlsx
+++ b/Mouse/MouseAdult_CellTypes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\freya\NAS\mgriswold\CellProfileLibrary\Mouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgriswold\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF9AAC6-AEC4-4F62-A10E-469BE078A4C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A756D2E-7FD7-4511-9F5D-8FAA48DC7B64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="7" xr2:uid="{EF3D0EE4-8FB4-4CD1-A1F7-226FF1ED9010}"/>
+    <workbookView xWindow="4950" yWindow="2265" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{EF3D0EE4-8FB4-4CD1-A1F7-226FF1ED9010}"/>
   </bookViews>
   <sheets>
     <sheet name="Bladder_MCA" sheetId="1" r:id="rId1"/>
@@ -18,30 +18,31 @@
     <sheet name="BoneMarrow_MCA" sheetId="3" r:id="rId3"/>
     <sheet name="Brain_AllenBrainAtlas" sheetId="4" r:id="rId4"/>
     <sheet name="Brain_AllenBrainAtlas_Class" sheetId="5" r:id="rId5"/>
-    <sheet name="ImmuneAtlas_ImmGen" sheetId="6" r:id="rId6"/>
-    <sheet name="ImmuneAtlas_ImmGen_Lineage" sheetId="7" r:id="rId7"/>
-    <sheet name="ImmuneAtlas_cellFamily_ImmGen" sheetId="27" r:id="rId8"/>
-    <sheet name="Kidney_MCA" sheetId="8" r:id="rId9"/>
-    <sheet name="Liver_MCA" sheetId="9" r:id="rId10"/>
-    <sheet name="Lung_MCA" sheetId="10" r:id="rId11"/>
-    <sheet name="MammaryGland_Involution_MCA" sheetId="11" r:id="rId12"/>
-    <sheet name="MammaryGland_Lactation_MCA" sheetId="12" r:id="rId13"/>
-    <sheet name="MammaryGland_Pregnancy_MCA" sheetId="13" r:id="rId14"/>
-    <sheet name="MammaryGland_Virgin_MCA" sheetId="14" r:id="rId15"/>
-    <sheet name="Muscle_MCA" sheetId="15" r:id="rId16"/>
-    <sheet name="Ovary_MCA" sheetId="16" r:id="rId17"/>
-    <sheet name="Pancreas_MCA" sheetId="17" r:id="rId18"/>
-    <sheet name="PeripheralBlood_MCA" sheetId="18" r:id="rId19"/>
-    <sheet name="Placenta_MCA" sheetId="19" r:id="rId20"/>
-    <sheet name="Prostate_MCA" sheetId="21" r:id="rId21"/>
-    <sheet name="SmallIntestine_MCA" sheetId="22" r:id="rId22"/>
-    <sheet name="Spleen_MCA" sheetId="23" r:id="rId23"/>
-    <sheet name="Stomach_MCA" sheetId="20" r:id="rId24"/>
-    <sheet name="Testis_MCA" sheetId="24" r:id="rId25"/>
-    <sheet name="Thymus_MCA" sheetId="26" r:id="rId26"/>
-    <sheet name="Uterus_MCA" sheetId="25" r:id="rId27"/>
+    <sheet name="Brain_MCA" sheetId="28" r:id="rId6"/>
+    <sheet name="ImmuneAtlas_ImmGen" sheetId="6" r:id="rId7"/>
+    <sheet name="ImmuneAtlas_ImmGen_Lineage" sheetId="7" r:id="rId8"/>
+    <sheet name="ImmuneAtlas_cellFamily_ImmGen" sheetId="27" r:id="rId9"/>
+    <sheet name="Kidney_MCA" sheetId="8" r:id="rId10"/>
+    <sheet name="Liver_MCA" sheetId="9" r:id="rId11"/>
+    <sheet name="Lung_MCA" sheetId="10" r:id="rId12"/>
+    <sheet name="MammaryGland_Involution_MCA" sheetId="11" r:id="rId13"/>
+    <sheet name="MammaryGland_Lactation_MCA" sheetId="12" r:id="rId14"/>
+    <sheet name="MammaryGland_Pregnancy_MCA" sheetId="13" r:id="rId15"/>
+    <sheet name="MammaryGland_Virgin_MCA" sheetId="14" r:id="rId16"/>
+    <sheet name="Muscle_MCA" sheetId="15" r:id="rId17"/>
+    <sheet name="Ovary_MCA" sheetId="16" r:id="rId18"/>
+    <sheet name="Pancreas_MCA" sheetId="17" r:id="rId19"/>
+    <sheet name="PeripheralBlood_MCA" sheetId="18" r:id="rId20"/>
+    <sheet name="Placenta_MCA" sheetId="19" r:id="rId21"/>
+    <sheet name="Prostate_MCA" sheetId="21" r:id="rId22"/>
+    <sheet name="SmallIntestine_MCA" sheetId="22" r:id="rId23"/>
+    <sheet name="Spleen_MCA" sheetId="23" r:id="rId24"/>
+    <sheet name="Stomach_MCA" sheetId="20" r:id="rId25"/>
+    <sheet name="Testis_MCA" sheetId="24" r:id="rId26"/>
+    <sheet name="Thymus_MCA" sheetId="26" r:id="rId27"/>
+    <sheet name="Uterus_MCA" sheetId="25" r:id="rId28"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="569">
   <si>
     <t>Main Cell Types</t>
   </si>
@@ -1730,6 +1731,42 @@
   </si>
   <si>
     <t>ImmGen Lineage</t>
+  </si>
+  <si>
+    <t>Astrocyte</t>
+  </si>
+  <si>
+    <t>Astrocyte_Atp1b2 high</t>
+  </si>
+  <si>
+    <t>Astrocyte_Mfe8 high</t>
+  </si>
+  <si>
+    <t>Astrocyte_Pla2g7 high</t>
+  </si>
+  <si>
+    <t>Granulocyte_Il33 high</t>
+  </si>
+  <si>
+    <t>Macrophage_Klf2 high</t>
+  </si>
+  <si>
+    <t>Myelinating oligodendrocyte</t>
+  </si>
+  <si>
+    <t>Neuron</t>
+  </si>
+  <si>
+    <t>Oligodendrocyte precursor</t>
+  </si>
+  <si>
+    <t>Pan-GABAergic Neuron</t>
+  </si>
+  <si>
+    <t>Schwann cell</t>
+  </si>
+  <si>
+    <t>Brain - MCA</t>
   </si>
 </sst>
 </file>
@@ -2337,6 +2374,282 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EEF57-B5B8-4D78-B3B2-42D185CE656B}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>268</v>
+      </c>
+      <c r="C19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>270</v>
+      </c>
+      <c r="C20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>280</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>281</v>
+      </c>
+      <c r="C30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>282</v>
+      </c>
+      <c r="C31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB956815-F334-4F7F-86CE-D4EEF7349043}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -2555,7 +2868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68C820-21F7-4933-9450-7EB4A96CC9B0}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -2855,7 +3168,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18332EA4-4892-4220-82A3-8FCC7889BB09}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -3071,7 +3384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EE7703-C29F-429C-AEFE-AFE16DBC3B8F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -3220,7 +3533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293175B3-E9D3-4891-955C-A545B22B3039}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3386,7 +3699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCE45EC-1854-47A6-8A21-1CB531DF28B1}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -3550,7 +3863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B615E9-DC7E-423E-95B6-2DD938DCC13E}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3703,7 +4016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B3BB5A-055A-4F48-9183-8C691CFA9515}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -3856,7 +4169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB4F90-763F-4E3F-A269-6706118906CA}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -4068,189 +4381,6 @@
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>280</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864E1DA6-CEDD-4307-BAFB-BA0D6D908F2B}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8</v>
       </c>
       <c r="B22" t="s">
         <v>280</v>
@@ -4449,6 +4579,189 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864E1DA6-CEDD-4307-BAFB-BA0D6D908F2B}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B7BA21-0A80-492F-B4EC-45FDEA9B6771}">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -4740,7 +5053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92F6DFB-87EC-4982-802A-3CB6EA7A1C94}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -4840,7 +5153,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDFD466-ED76-42E4-9A65-C8FF1E75DAB7}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5046,7 +5359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54525862-2259-4188-B666-A82E90BAAAA9}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -5174,7 +5487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791BEBCD-EE0E-40EF-8CC2-BB9FA5D1BFC0}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -5351,7 +5664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254D654-1F29-4824-AB6E-728ECFB0A4A7}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -5535,7 +5848,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276ED048-DC5A-4251-B79A-3B7CBE2B5F74}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5651,7 +5964,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C902E0-24D1-46E1-93F8-7EAA1C41C717}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -5847,7 +6160,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C16"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6624,6 +6937,159 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A236248-5D66-4FFF-B5A3-BB6E90DCF014}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>557</v>
+      </c>
+      <c r="C3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C7" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>563</v>
+      </c>
+      <c r="C11" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>564</v>
+      </c>
+      <c r="C12" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>565</v>
+      </c>
+      <c r="C13" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>566</v>
+      </c>
+      <c r="C14" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>567</v>
+      </c>
+      <c r="C15" t="s">
+        <v>567</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB6C12C-72E0-4C23-90BA-03E5ADDFA956}">
   <dimension ref="A1:C78"/>
   <sheetViews>
@@ -7288,7 +7754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C03B65-E18B-4D7B-A426-08AC6386E6E8}">
   <dimension ref="A1:C78"/>
   <sheetViews>
@@ -7759,11 +8225,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186C9533-05F4-494A-B604-9D0B68B427BD}">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -8058,280 +8524,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EEF57-B5B8-4D78-B3B2-42D185CE656B}">
-  <dimension ref="A1:C31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>250</v>
-      </c>
-      <c r="C4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>255</v>
-      </c>
-      <c r="C8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C14" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>9</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>268</v>
-      </c>
-      <c r="C19" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>270</v>
-      </c>
-      <c r="C20" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>13</v>
-      </c>
-      <c r="B24" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>280</v>
-      </c>
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>15</v>
-      </c>
-      <c r="B30" t="s">
-        <v>281</v>
-      </c>
-      <c r="C30" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>16</v>
-      </c>
-      <c r="B31" t="s">
-        <v>282</v>
-      </c>
-      <c r="C31" t="s">
-        <v>282</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update with sheet for colon celltypes
</commit_message>
<xml_diff>
--- a/Mouse/MouseAdult_CellTypes.xlsx
+++ b/Mouse/MouseAdult_CellTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgriswold\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcguire\Desktop\smi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A756D2E-7FD7-4511-9F5D-8FAA48DC7B64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F781E2-7202-4BDD-B4F0-23063E9B1DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="2265" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{EF3D0EE4-8FB4-4CD1-A1F7-226FF1ED9010}"/>
+    <workbookView xWindow="1515" yWindow="810" windowWidth="22080" windowHeight="11385" firstSheet="3" activeTab="6" xr2:uid="{EF3D0EE4-8FB4-4CD1-A1F7-226FF1ED9010}"/>
   </bookViews>
   <sheets>
     <sheet name="Bladder_MCA" sheetId="1" r:id="rId1"/>
@@ -19,30 +19,31 @@
     <sheet name="Brain_AllenBrainAtlas" sheetId="4" r:id="rId4"/>
     <sheet name="Brain_AllenBrainAtlas_Class" sheetId="5" r:id="rId5"/>
     <sheet name="Brain_MCA" sheetId="28" r:id="rId6"/>
-    <sheet name="ImmuneAtlas_ImmGen" sheetId="6" r:id="rId7"/>
-    <sheet name="ImmuneAtlas_ImmGen_Lineage" sheetId="7" r:id="rId8"/>
-    <sheet name="ImmuneAtlas_cellFamily_ImmGen" sheetId="27" r:id="rId9"/>
-    <sheet name="Kidney_MCA" sheetId="8" r:id="rId10"/>
-    <sheet name="Liver_MCA" sheetId="9" r:id="rId11"/>
-    <sheet name="Lung_MCA" sheetId="10" r:id="rId12"/>
-    <sheet name="MammaryGland_Involution_MCA" sheetId="11" r:id="rId13"/>
-    <sheet name="MammaryGland_Lactation_MCA" sheetId="12" r:id="rId14"/>
-    <sheet name="MammaryGland_Pregnancy_MCA" sheetId="13" r:id="rId15"/>
-    <sheet name="MammaryGland_Virgin_MCA" sheetId="14" r:id="rId16"/>
-    <sheet name="Muscle_MCA" sheetId="15" r:id="rId17"/>
-    <sheet name="Ovary_MCA" sheetId="16" r:id="rId18"/>
-    <sheet name="Pancreas_MCA" sheetId="17" r:id="rId19"/>
-    <sheet name="PeripheralBlood_MCA" sheetId="18" r:id="rId20"/>
-    <sheet name="Placenta_MCA" sheetId="19" r:id="rId21"/>
-    <sheet name="Prostate_MCA" sheetId="21" r:id="rId22"/>
-    <sheet name="SmallIntestine_MCA" sheetId="22" r:id="rId23"/>
-    <sheet name="Spleen_MCA" sheetId="23" r:id="rId24"/>
-    <sheet name="Stomach_MCA" sheetId="20" r:id="rId25"/>
-    <sheet name="Testis_MCA" sheetId="24" r:id="rId26"/>
-    <sheet name="Thymus_MCA" sheetId="26" r:id="rId27"/>
-    <sheet name="Uterus_MCA" sheetId="25" r:id="rId28"/>
+    <sheet name="Colon_SCP2038" sheetId="29" r:id="rId7"/>
+    <sheet name="ImmuneAtlas_ImmGen" sheetId="6" r:id="rId8"/>
+    <sheet name="ImmuneAtlas_ImmGen_Lineage" sheetId="7" r:id="rId9"/>
+    <sheet name="ImmuneAtlas_cellFamily_ImmGen" sheetId="27" r:id="rId10"/>
+    <sheet name="Kidney_MCA" sheetId="8" r:id="rId11"/>
+    <sheet name="Liver_MCA" sheetId="9" r:id="rId12"/>
+    <sheet name="Lung_MCA" sheetId="10" r:id="rId13"/>
+    <sheet name="MammaryGland_Involution_MCA" sheetId="11" r:id="rId14"/>
+    <sheet name="MammaryGland_Lactation_MCA" sheetId="12" r:id="rId15"/>
+    <sheet name="MammaryGland_Pregnancy_MCA" sheetId="13" r:id="rId16"/>
+    <sheet name="MammaryGland_Virgin_MCA" sheetId="14" r:id="rId17"/>
+    <sheet name="Muscle_MCA" sheetId="15" r:id="rId18"/>
+    <sheet name="Ovary_MCA" sheetId="16" r:id="rId19"/>
+    <sheet name="Pancreas_MCA" sheetId="17" r:id="rId20"/>
+    <sheet name="PeripheralBlood_MCA" sheetId="18" r:id="rId21"/>
+    <sheet name="Placenta_MCA" sheetId="19" r:id="rId22"/>
+    <sheet name="Prostate_MCA" sheetId="21" r:id="rId23"/>
+    <sheet name="SmallIntestine_MCA" sheetId="22" r:id="rId24"/>
+    <sheet name="Spleen_MCA" sheetId="23" r:id="rId25"/>
+    <sheet name="Stomach_MCA" sheetId="20" r:id="rId26"/>
+    <sheet name="Testis_MCA" sheetId="24" r:id="rId27"/>
+    <sheet name="Thymus_MCA" sheetId="26" r:id="rId28"/>
+    <sheet name="Uterus_MCA" sheetId="25" r:id="rId29"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="578">
   <si>
     <t>Main Cell Types</t>
   </si>
@@ -1767,6 +1768,33 @@
   </si>
   <si>
     <t>Brain - MCA</t>
+  </si>
+  <si>
+    <t>Colon - SCP2038</t>
+  </si>
+  <si>
+    <t>colon.epithelial.cell</t>
+  </si>
+  <si>
+    <t>B.cell</t>
+  </si>
+  <si>
+    <t>lymphocyte</t>
+  </si>
+  <si>
+    <t>macrophage</t>
+  </si>
+  <si>
+    <t>mast.cell</t>
+  </si>
+  <si>
+    <t>granulocyte</t>
+  </si>
+  <si>
+    <t>fibroblast</t>
+  </si>
+  <si>
+    <t>endothelial.cell</t>
   </si>
 </sst>
 </file>
@@ -2374,11 +2402,312 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186C9533-05F4-494A-B604-9D0B68B427BD}">
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>246</v>
+      </c>
+      <c r="C37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" t="s">
+        <v>247</v>
+      </c>
+      <c r="C38" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
+        <v>248</v>
+      </c>
+      <c r="C42" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>214</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85EEF57-B5B8-4D78-B3B2-42D185CE656B}">
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,7 +2978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB956815-F334-4F7F-86CE-D4EEF7349043}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -2868,7 +3197,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC68C820-21F7-4933-9450-7EB4A96CC9B0}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -3168,7 +3497,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18332EA4-4892-4220-82A3-8FCC7889BB09}">
   <dimension ref="A1:C25"/>
   <sheetViews>
@@ -3384,7 +3713,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78EE7703-C29F-429C-AEFE-AFE16DBC3B8F}">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -3533,7 +3862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293175B3-E9D3-4891-955C-A545B22B3039}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -3699,7 +4028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCE45EC-1854-47A6-8A21-1CB531DF28B1}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -3863,7 +4192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32B615E9-DC7E-423E-95B6-2DD938DCC13E}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -4016,7 +4345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B3BB5A-055A-4F48-9183-8C691CFA9515}">
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -4162,231 +4491,6 @@
       </c>
       <c r="C16" t="s">
         <v>406</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB4F90-763F-4E3F-A269-6706118906CA}">
-  <dimension ref="A1:C22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:C22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C3" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>410</v>
-      </c>
-      <c r="C5" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>412</v>
-      </c>
-      <c r="C7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>414</v>
-      </c>
-      <c r="C8" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C9" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>421</v>
-      </c>
-      <c r="C15" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
-        <v>290</v>
-      </c>
-      <c r="C16" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>13</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>14</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>15</v>
-      </c>
-      <c r="B22" t="s">
-        <v>280</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -4579,6 +4683,231 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1DB4F90-763F-4E3F-A269-6706118906CA}">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>408</v>
+      </c>
+      <c r="C3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C7" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>414</v>
+      </c>
+      <c r="C8" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>416</v>
+      </c>
+      <c r="C9" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>421</v>
+      </c>
+      <c r="C15" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>290</v>
+      </c>
+      <c r="C16" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864E1DA6-CEDD-4307-BAFB-BA0D6D908F2B}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -4761,7 +5090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B7BA21-0A80-492F-B4EC-45FDEA9B6771}">
   <dimension ref="A1:C27"/>
   <sheetViews>
@@ -5053,7 +5382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92F6DFB-87EC-4982-802A-3CB6EA7A1C94}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -5153,7 +5482,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBDFD466-ED76-42E4-9A65-C8FF1E75DAB7}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -5359,7 +5688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54525862-2259-4188-B666-A82E90BAAAA9}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -5487,7 +5816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791BEBCD-EE0E-40EF-8CC2-BB9FA5D1BFC0}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -5664,7 +5993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D254D654-1F29-4824-AB6E-728ECFB0A4A7}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -5848,7 +6177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276ED048-DC5A-4251-B79A-3B7CBE2B5F74}">
   <dimension ref="A1:C10"/>
   <sheetViews>
@@ -5964,7 +6293,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3C902E0-24D1-46E1-93F8-7EAA1C41C717}">
   <dimension ref="A1:C20"/>
   <sheetViews>
@@ -6940,8 +7269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A236248-5D66-4FFF-B5A3-BB6E90DCF014}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7090,6 +7419,139 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{365D35FC-3E88-491D-BBA7-E1EBB6F502F4}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>570</v>
+      </c>
+      <c r="C3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>571</v>
+      </c>
+      <c r="C4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>572</v>
+      </c>
+      <c r="C5" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>573</v>
+      </c>
+      <c r="C6" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>574</v>
+      </c>
+      <c r="C8" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>575</v>
+      </c>
+      <c r="C9" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>576</v>
+      </c>
+      <c r="C10" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>577</v>
+      </c>
+      <c r="C11" t="s">
+        <v>577</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB6C12C-72E0-4C23-90BA-03E5ADDFA956}">
   <dimension ref="A1:C78"/>
   <sheetViews>
@@ -7754,7 +8216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87C03B65-E18B-4D7B-A426-08AC6386E6E8}">
   <dimension ref="A1:C78"/>
   <sheetViews>
@@ -8223,305 +8685,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186C9533-05F4-494A-B604-9D0B68B427BD}">
-  <dimension ref="A1:C44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>241</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>242</v>
-      </c>
-      <c r="C24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>243</v>
-      </c>
-      <c r="C25" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s">
-        <v>171</v>
-      </c>
-      <c r="C26" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>6</v>
-      </c>
-      <c r="B28" t="s">
-        <v>244</v>
-      </c>
-      <c r="C28" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>245</v>
-      </c>
-      <c r="C30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>8</v>
-      </c>
-      <c r="B37" t="s">
-        <v>246</v>
-      </c>
-      <c r="C37" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>9</v>
-      </c>
-      <c r="B38" t="s">
-        <v>247</v>
-      </c>
-      <c r="C38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>10</v>
-      </c>
-      <c r="B42" t="s">
-        <v>248</v>
-      </c>
-      <c r="C42" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C44" t="s">
-        <v>214</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>